<commit_message>
foglio excel metriche processo
</commit_message>
<xml_diff>
--- a/DocEsterna/PianoDiQualifica/Images/graficiGulpease nuovo.xlsx
+++ b/DocEsterna/PianoDiQualifica/Images/graficiGulpease nuovo.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zenma\Desktop\Desktop Marco\UNIPD\Ingegneria del Software\CodeBusters-Docs\DocEsterna\PianoDiQualifica\Images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51A58963-6C47-400A-91CE-50990BAA46D0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF46A92F-282F-43E2-A820-226973102A7E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{F0DD3E61-CE4D-4D6D-8EBE-270C615506EB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F0DD3E61-CE4D-4D6D-8EBE-270C615506EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
-    <sheet name="Metriche processi" sheetId="2" r:id="rId2"/>
-    <sheet name="Metriche Software" sheetId="3" r:id="rId3"/>
-    <sheet name="Metriche Documenti" sheetId="4" r:id="rId4"/>
+    <sheet name="Metriche Software" sheetId="3" r:id="rId2"/>
+    <sheet name="Metriche Documenti" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="38">
   <si>
     <t>Analisi</t>
   </si>
@@ -63,9 +62,6 @@
     <t>Media verbali</t>
   </si>
   <si>
-    <t>Metriche processi</t>
-  </si>
-  <si>
     <t>Incremento 1</t>
   </si>
   <si>
@@ -88,42 +84,6 @@
   </si>
   <si>
     <t>Incremento 8</t>
-  </si>
-  <si>
-    <t>Schedule Variance</t>
-  </si>
-  <si>
-    <t>Budget Variance</t>
-  </si>
-  <si>
-    <t>Budget at Completion</t>
-  </si>
-  <si>
-    <t>Earned Value</t>
-  </si>
-  <si>
-    <t>Planned Value</t>
-  </si>
-  <si>
-    <t>Requirements stability index</t>
-  </si>
-  <si>
-    <t>Satisfied obligatory requirements</t>
-  </si>
-  <si>
-    <t>Code Coverage</t>
-  </si>
-  <si>
-    <t>Passed test cases percentage</t>
-  </si>
-  <si>
-    <t>Failed test cases Percentage</t>
-  </si>
-  <si>
-    <t>Quality Metrics Satisfied</t>
-  </si>
-  <si>
-    <t>Non-calculated Risk</t>
   </si>
   <si>
     <t>Copertura requisiti</t>
@@ -254,10 +214,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -7905,7 +7865,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{351464DA-C1FD-4F90-B8EF-3877AE8C241A}">
   <dimension ref="A1:H110"/>
   <sheetViews>
-    <sheetView zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
@@ -8156,132 +8116,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{687C4B70-CAB6-4B77-844E-3060F7E9865F}">
-  <dimension ref="A1:J13"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="31.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="10" width="12.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="2"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="2"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="2"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="2"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="2"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" s="2"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" s="2"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="2"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" s="2"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11" s="2"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12" s="2"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B13" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54E02C8E-8587-4B94-82DE-105FC5F151F1}">
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:J1"/>
+      <selection sqref="A1:J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8292,74 +8131,74 @@
   <sheetData>
     <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -8367,12 +8206,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB3B5200-58CF-498E-834C-4CD9DF998495}">
   <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:A20"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8382,74 +8221,74 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B1" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
+      <c r="B1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
       <c r="F1" s="3"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
     </row>
     <row r="2" spans="1:14" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -8459,7 +8298,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -8474,66 +8313,66 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="21" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="G12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="I12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I12" s="2" t="s">
+      <c r="J12" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="J12" s="2" t="s">
+      <c r="K12" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="K12" s="2" t="s">
+      <c r="L12" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="L12" s="2" t="s">
+      <c r="M12" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="M12" s="2" t="s">
+      <c r="N12" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="N12" s="2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -8543,7 +8382,7 @@
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
@@ -8558,7 +8397,7 @@
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bozza metriche software / gulpease?? / errori
</commit_message>
<xml_diff>
--- a/DocEsterna/PianoDiQualifica/Images/graficiGulpease nuovo.xlsx
+++ b/DocEsterna/PianoDiQualifica/Images/graficiGulpease nuovo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\swe\Progetto!\CodeBusters-Docs\DocEsterna\PianoDiQualifica\Images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A2D6A52-FF6C-4A1A-9736-664405D56D57}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF33F39F-99FA-4B9D-B700-198F0B369604}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F0DD3E61-CE4D-4D6D-8EBE-270C615506EB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{F0DD3E61-CE4D-4D6D-8EBE-270C615506EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="49">
   <si>
     <t>Analisi</t>
   </si>
@@ -168,6 +168,21 @@
   </si>
   <si>
     <t>Piano di Progetto</t>
+  </si>
+  <si>
+    <t>(linee commenti / linee codice) * 100</t>
+  </si>
+  <si>
+    <t>numero di click necessario per la funzionalità</t>
+  </si>
+  <si>
+    <t>numero di minuti che un utente usa per capire come funzia</t>
+  </si>
+  <si>
+    <t>percentuale test falliti</t>
+  </si>
+  <si>
+    <t>(1 - requisiti manc/requisiti tot) *100</t>
   </si>
 </sst>
 </file>
@@ -889,6 +904,1431 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="it-IT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="it-IT"/>
+              <a:t>Errori ortografici</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="it-IT"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Metriche Documenti'!$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Analisi dei requisiti</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Metriche Documenti'!$B$12:$C$12</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>RR</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>RP</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Metriche Documenti'!$B$13:$C$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-850C-4941-8CA6-5D6B3DC503A9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Metriche Documenti'!$A$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Piano di progetto</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Metriche Documenti'!$B$12:$C$12</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>RR</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>RP</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Metriche Documenti'!$B$14:$C$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-850C-4941-8CA6-5D6B3DC503A9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Metriche Documenti'!$A$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Piano di qualifica</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Metriche Documenti'!$B$12:$C$12</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>RR</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>RP</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Metriche Documenti'!$B$15:$C$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-850C-4941-8CA6-5D6B3DC503A9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Metriche Documenti'!$A$16</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Glossario</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Metriche Documenti'!$B$12:$C$12</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>RR</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>RP</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Metriche Documenti'!$B$16:$C$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-850C-4941-8CA6-5D6B3DC503A9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Metriche Documenti'!$A$17</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Norme di progetto</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Metriche Documenti'!$B$12:$C$12</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>RR</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>RP</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Metriche Documenti'!$B$17:$C$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-850C-4941-8CA6-5D6B3DC503A9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Metriche Documenti'!$A$18</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Studio di fattibilità</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Metriche Documenti'!$B$12:$C$12</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>RR</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>RP</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Metriche Documenti'!$B$18:$C$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-850C-4941-8CA6-5D6B3DC503A9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Metriche Documenti'!$A$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Media verbali</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Metriche Documenti'!$B$12:$C$12</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>RR</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>RP</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Metriche Documenti'!$B$19:$C$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-850C-4941-8CA6-5D6B3DC503A9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Metriche Documenti'!$A$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Accettazione</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Metriche Documenti'!$B$12:$C$12</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>RR</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>RP</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Metriche Documenti'!$B$20:$C$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-850C-4941-8CA6-5D6B3DC503A9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="614442680"/>
+        <c:axId val="614446520"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="614442680"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="614446520"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="614446520"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="614442680"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="it-IT"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="it-IT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -910,6 +2350,47 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{85665F02-754E-4F97-AC62-692F12C3049D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>91440</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>3810</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>320040</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>3810</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Grafico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4EF4B671-6DB8-474F-9E5B-241A8B1890DB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1229,7 +2710,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{351464DA-C1FD-4F90-B8EF-3877AE8C241A}">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
+    <sheetView zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
       <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
@@ -1325,10 +2806,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54E02C8E-8587-4B94-82DE-105FC5F151F1}">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1338,7 +2819,7 @@
     <col min="12" max="12" width="34.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>36</v>
       </c>
@@ -1370,15 +2851,18 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>15</v>
       </c>
       <c r="L2" t="s">
         <v>40</v>
       </c>
+      <c r="M2" t="s">
+        <v>48</v>
+      </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>16</v>
       </c>
@@ -1387,38 +2871,51 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="L5" t="s">
+        <v>44</v>
+      </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="L7" t="s">
+        <v>45</v>
+      </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>21</v>
       </c>
+      <c r="L8" t="s">
+        <v>46</v>
+      </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>22</v>
+      </c>
+      <c r="L9" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1427,7 +2924,7 @@
   <dimension ref="A1:N20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1499,9 +2996,6 @@
       <c r="E3">
         <v>70</v>
       </c>
-      <c r="F3">
-        <v>90</v>
-      </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
@@ -1510,9 +3004,6 @@
       <c r="E4">
         <v>65</v>
       </c>
-      <c r="F4">
-        <v>81</v>
-      </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
@@ -1521,9 +3012,6 @@
       <c r="E5">
         <v>67</v>
       </c>
-      <c r="F5">
-        <v>86</v>
-      </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
@@ -1532,9 +3020,6 @@
       <c r="E6">
         <v>71</v>
       </c>
-      <c r="F6">
-        <v>80</v>
-      </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
@@ -1543,9 +3028,6 @@
       <c r="E7">
         <v>77</v>
       </c>
-      <c r="F7">
-        <v>80</v>
-      </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
@@ -1554,9 +3036,6 @@
       <c r="E8">
         <v>73</v>
       </c>
-      <c r="F8">
-        <v>87</v>
-      </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
@@ -1565,28 +3044,10 @@
       <c r="E9">
         <v>70</v>
       </c>
-      <c r="F9">
-        <v>91</v>
-      </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="B10">
-        <v>80</v>
-      </c>
-      <c r="C10">
-        <v>80</v>
-      </c>
-      <c r="D10">
-        <v>80</v>
-      </c>
-      <c r="E10">
-        <v>80</v>
-      </c>
-      <c r="F10">
-        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="21" x14ac:dyDescent="0.4">
@@ -1729,5 +3190,6 @@
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>